<commit_message>
bahan exporting user - update
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Ekspor Users/KEPEGAWAIAN x SIMRSMU - BACKUP.xlsx
+++ b/project/kepegawaian/Ekspor Users/KEPEGAWAIAN x SIMRSMU - BACKUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\Ekspor Users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B595CED5-7AF5-450D-8874-65A6DA1B1AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB905922-0FF4-49C0-BE7C-D3EB8FCE2EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="16230" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PENGGUNA" sheetId="1" r:id="rId1"/>
@@ -8731,6 +8731,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8803,7 +8804,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9194,7 +9194,7 @@
   </sheetPr>
   <dimension ref="A1:BU365"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
@@ -9317,17 +9317,17 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="29" t="s">
         <v>694</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -9400,17 +9400,17 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="27" t="s">
         <v>698</v>
       </c>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
@@ -9483,15 +9483,15 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -9564,15 +9564,15 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
@@ -9645,15 +9645,15 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -9726,15 +9726,15 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -10746,11 +10746,11 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="17" t="s">
+      <c r="L20" s="18" t="s">
         <v>695</v>
       </c>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="20"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
@@ -10829,9 +10829,9 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="22"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="23"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -10910,9 +10910,9 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="26"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
@@ -38673,34 +38673,34 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="17" t="s">
         <v>2695</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="17" t="s">
         <v>2696</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="17" t="s">
         <v>2697</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="17" t="s">
         <v>2698</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="17" t="s">
         <v>2699</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="17" t="s">
         <v>2700</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="17" t="s">
         <v>2701</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="17" t="s">
         <v>2702</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="17" t="s">
         <v>2703</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="17" t="s">
         <v>690</v>
       </c>
     </row>
@@ -50711,8 +50711,8 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50725,21 +50725,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="33"/>
+      <c r="D1" s="34" t="s">
         <v>686</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="G1" s="35" t="s">
+      <c r="E1" s="35"/>
+      <c r="G1" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="14" t="s">
@@ -50754,23 +50754,26 @@
       <c r="E2" s="15" t="s">
         <v>679</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="39" t="s">
         <v>691</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9">
-        <v>1</v>
+        <v>154</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>697</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3" s="9">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>687</v>
@@ -50778,13 +50781,16 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="9">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>681</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
       <c r="D4" s="9">
-        <v>2</v>
+        <v>151</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>688</v>
@@ -50792,13 +50798,16 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1">
       <c r="A5" s="9">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>682</v>
       </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
       <c r="D5" s="12">
-        <v>3</v>
+        <v>152</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>689</v>
@@ -50806,28 +50815,37 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="9">
-        <v>4</v>
+        <v>147</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>683</v>
       </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="9">
-        <v>5</v>
+        <v>148</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>684</v>
       </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1">
       <c r="A8" s="12">
-        <v>6</v>
+        <v>149</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>685</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:11">

</xml_diff>